<commit_message>
Add a weekly validation case of window AC
</commit_message>
<xml_diff>
--- a/Buildings/Resources/Data/Fluid/ZoneEquipment/WindowAC/fan_curve_calculations.xlsx
+++ b/Buildings/Resources/Data/Fluid/ZoneEquipment/WindowAC/fan_curve_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\buildings_library\buildings_library_pnnl\Buildings\Resources\Data\Fluid\ZoneEquipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\modelica-buildings\Buildings\Resources\Data\Fluid\ZoneEquipment\WindowAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF69824-0291-467A-A3B6-0507F7510C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B5B344-F013-4A70-A354-A06D4D5CF901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5700" windowWidth="18240" windowHeight="28440" xr2:uid="{394E563C-5E41-4DF9-8874-6D3AA803DB52}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{394E563C-5E41-4DF9-8874-6D3AA803DB52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,17 +436,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102010AF-90B6-4F8D-82A0-2B238E4FDE5C}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,11 +457,11 @@
         <v>9</v>
       </c>
       <c r="E1">
-        <f>0.419361</f>
-        <v>0.41936099999999998</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <f>0.43157</f>
+        <v>0.43157000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,10 +473,10 @@
       </c>
       <c r="E2">
         <f>E3*E1</f>
-        <v>31.452074999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32.367750000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -490,7 +490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +498,7 @@
         <v>1.0092000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -523,7 +523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <f>0</f>
         <v>0</v>
@@ -538,17 +538,17 @@
       </c>
       <c r="D8" s="1">
         <f>C8*$E$2</f>
-        <v>2.2151696422499998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.2796606325000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <f>0.1*$E$1</f>
-        <v>4.1936100000000004E-2</v>
+        <v>4.3157000000000001E-2</v>
       </c>
       <c r="B9">
         <f t="shared" ref="B9:B18" si="0">A9/$E$1</f>
-        <v>0.10000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C18" si="1">$B$1 + $B$2*B9 + $B$3*B9^2 + $B$4*B9^3 + $B$5*B9^4</f>
@@ -556,21 +556,21 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:D18" si="2">C9*$E$2</f>
-        <v>3.3139038494699999</v>
+        <v>3.4103826639000001</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E8:E17" si="3">$E$3*($B$18^2)/(B9^2)</f>
-        <v>7499.9999999999973</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E9:E17" si="3">$E$3*($B$18^2)/(B9^2)</f>
+        <v>7499.9999999999982</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <f>0.2*$E$1</f>
-        <v>8.3872200000000008E-2</v>
+        <v>8.6314000000000002E-2</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.20000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -578,17 +578,17 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>4.3131865955400004</v>
+        <v>4.4387578698000008</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>1874.9999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1874.9999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <f>0.3*$E$1</f>
-        <v>0.12580829999999998</v>
+        <v>0.129471</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -600,39 +600,39 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>5.403466485</v>
+        <v>5.5607794500000001</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
         <v>833.33333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <f>0.4*$E$1</f>
-        <v>0.16774440000000002</v>
+        <v>0.172628</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.40000000000000008</v>
+        <v>0.4</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0.21541320000000005</v>
+        <v>0.21541320000000003</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>6.7751921223900009</v>
+        <v>6.9724406043000009</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>468.74999999999983</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>468.74999999999989</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <f>0.5*$E$1</f>
-        <v>0.20968049999999999</v>
+        <v>0.215785</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -644,17 +644,17 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>8.6188121122499997</v>
+        <v>8.8697345325000008</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <f>0.6*$E$1</f>
-        <v>0.25161659999999997</v>
+        <v>0.25894200000000001</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -666,61 +666,61 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>11.124775059120001</v>
+        <v>11.448654434400002</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
         <v>208.33333333333334</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <f>0.7*$E$1</f>
-        <v>0.29355269999999994</v>
+        <v>0.30209900000000001</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0.69999999999999984</v>
+        <v>0.7</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.46049519999999983</v>
+        <v>0.46049519999999999</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
-        <v>14.483529567539993</v>
+        <v>14.9051935098</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>153.06122448979599</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153.06122448979593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <f>0.8*$E$1</f>
-        <v>0.33548880000000003</v>
+        <v>0.34525600000000001</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>0.80000000000000016</v>
+        <v>0.8</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.60045400000000015</v>
+        <v>0.60045400000000004</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>18.885524242050003</v>
+        <v>19.435344958500004</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>117.18749999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117.18749999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <f>0.9*$E$1</f>
-        <v>0.37742490000000001</v>
+        <v>0.38841300000000001</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -732,17 +732,17 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>24.521207687190007</v>
+        <v>25.235101980300009</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
         <v>92.592592592592581</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <f>1*$E$1</f>
-        <v>0.41936099999999998</v>
+        <v>0.43157000000000001</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -754,7 +754,7 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="2"/>
-        <v>31.581028507500005</v>
+        <v>32.500457775000008</v>
       </c>
       <c r="E18">
         <f>$E$3*($B$18^2)/(B18^2)</f>

</xml_diff>